<commit_message>
Mise a jour des attribue
</commit_message>
<xml_diff>
--- a/Chezjombi/Fonctionnalite.xlsx
+++ b/Chezjombi/Fonctionnalite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t xml:space="preserve">Client </t>
   </si>
@@ -96,6 +96,60 @@
   </si>
   <si>
     <t>Simulateur d'interraction dans un bar</t>
+  </si>
+  <si>
+    <t>Fonction/Personnage</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Serveur</t>
+  </si>
+  <si>
+    <t>Patron</t>
+  </si>
+  <si>
+    <t>Surnom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argent en poche </t>
+  </si>
+  <si>
+    <t>Charme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prenom </t>
+  </si>
+  <si>
+    <t>Attribu/Personnage</t>
+  </si>
+  <si>
+    <t>Boisson preferée</t>
+  </si>
+  <si>
+    <t>Sexe</t>
+  </si>
+  <si>
+    <t>Taille biceps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agilite </t>
+  </si>
+  <si>
+    <t>Boisson secours</t>
+  </si>
+  <si>
+    <t>Humain</t>
+  </si>
+  <si>
+    <t>Degres alcoolemie</t>
+  </si>
+  <si>
+    <t>Commun</t>
+  </si>
+  <si>
+    <t>Non Commun</t>
   </si>
 </sst>
 </file>
@@ -137,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -164,6 +218,21 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -278,30 +347,73 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,197 +728,394 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F20"/>
+  <dimension ref="B1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="21.15234375" customWidth="1"/>
     <col min="3" max="3" width="11.07421875" customWidth="1"/>
+    <col min="8" max="8" width="18.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-    </row>
-    <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C3" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="6"/>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B7" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B8" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="7"/>
+      <c r="H7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B9" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="6"/>
+      <c r="H8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B10" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="7"/>
+      <c r="H9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B11" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="7"/>
+      <c r="H10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B12" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="6"/>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B13" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="6"/>
+      <c r="H12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B14" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="H13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B15" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="7"/>
+      <c r="H14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B15" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B16" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="7"/>
+      <c r="H15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B17" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="7"/>
+      <c r="H16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B18" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6"/>
+      <c r="H17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="9"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B19" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="7"/>
+      <c r="H18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B19" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B20" t="s">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="6"/>
+      <c r="H19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="9"/>
+      <c r="H20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B23" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B24" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="6"/>
+      <c r="H24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B25" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="7"/>
+      <c r="H25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B26" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="6"/>
+      <c r="H26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B27" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="6"/>
+      <c r="H27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B28" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="7"/>
+      <c r="H28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B29" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="6"/>
+      <c r="H29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B30" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="6"/>
+      <c r="H30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B31" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="6"/>
+      <c r="H31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="9"/>
+      <c r="H32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B33" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="1"/>
+      <c r="H33" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Mise a jour Attribue
</commit_message>
<xml_diff>
--- a/Chezjombi/Fonctionnalite.xlsx
+++ b/Chezjombi/Fonctionnalite.xlsx
@@ -38,9 +38,6 @@
     <t xml:space="preserve">Patron </t>
   </si>
   <si>
-    <t>Parler</t>
-  </si>
-  <si>
     <t>Boire</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t>Non Commun</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -743,10 +743,10 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>23</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
@@ -755,7 +755,7 @@
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>0</v>
@@ -770,351 +770,351 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B4" s="18" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="6"/>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B5" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="6"/>
       <c r="H5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B6" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B7" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="7"/>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="6"/>
       <c r="H8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B9" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="5"/>
       <c r="F9" s="7"/>
       <c r="H9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B10" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="7"/>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B11" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="5"/>
       <c r="E11" s="3"/>
       <c r="F11" s="6"/>
       <c r="H11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B12" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="5"/>
       <c r="E12" s="3"/>
       <c r="F12" s="6"/>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B13" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="3"/>
       <c r="E13" s="5"/>
       <c r="F13" s="6"/>
       <c r="H13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B14" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="3"/>
       <c r="F14" s="7"/>
       <c r="H14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B15" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="3"/>
       <c r="F15" s="7"/>
       <c r="H15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B16" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="3"/>
       <c r="F16" s="7"/>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B17" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
       <c r="H17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B18" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="5"/>
       <c r="F18" s="7"/>
       <c r="H18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B19" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="3"/>
       <c r="F19" s="6"/>
       <c r="H19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="9"/>
       <c r="H20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="23" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B23" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>26</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>2</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B24" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="6"/>
       <c r="H24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B25" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="5"/>
       <c r="E25" s="3"/>
       <c r="F25" s="7"/>
       <c r="H25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B26" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="5"/>
       <c r="E26" s="3"/>
       <c r="F26" s="6"/>
       <c r="H26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B27" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="5"/>
       <c r="E27" s="3"/>
       <c r="F27" s="6"/>
       <c r="H27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B28" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="7"/>
       <c r="H28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B29" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="6"/>
       <c r="H29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B30" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="6"/>
       <c r="H30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B31" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="6"/>
       <c r="H31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B32" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="16"/>
       <c r="E32" s="8"/>
       <c r="F32" s="9"/>
       <c r="H32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B33" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="1"/>
       <c r="H33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementation de la nouvelle architecture
</commit_message>
<xml_diff>
--- a/Chezjombi/Fonctionnalite.xlsx
+++ b/Chezjombi/Fonctionnalite.xlsx
@@ -38,6 +38,9 @@
     <t xml:space="preserve">Patron </t>
   </si>
   <si>
+    <t>Parler</t>
+  </si>
+  <si>
     <t>Boire</t>
   </si>
   <si>
@@ -147,9 +150,6 @@
   </si>
   <si>
     <t>Non Commun</t>
-  </si>
-  <si>
-    <t>S</t>
   </si>
 </sst>
 </file>
@@ -731,7 +731,7 @@
   <dimension ref="B1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -743,10 +743,10 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
@@ -755,7 +755,7 @@
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>0</v>
@@ -770,351 +770,351 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B4" s="18" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="6"/>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B5" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="6"/>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B6" s="14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B7" s="14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="7"/>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8" s="14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="6"/>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B9" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="5"/>
       <c r="F9" s="7"/>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B10" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="7"/>
       <c r="H10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B11" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="5"/>
       <c r="E11" s="3"/>
       <c r="F11" s="6"/>
       <c r="H11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B12" s="14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="5"/>
       <c r="E12" s="3"/>
       <c r="F12" s="6"/>
       <c r="H12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B13" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="3"/>
       <c r="E13" s="5"/>
       <c r="F13" s="6"/>
       <c r="H13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B14" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="3"/>
       <c r="F14" s="7"/>
       <c r="H14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B15" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="3"/>
       <c r="F15" s="7"/>
       <c r="H15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B16" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="3"/>
       <c r="F16" s="7"/>
       <c r="H16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B17" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
       <c r="H17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B18" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="5"/>
       <c r="F18" s="7"/>
       <c r="H18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B19" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="3"/>
       <c r="F19" s="6"/>
       <c r="H19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="9"/>
       <c r="H20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="23" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B23" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>2</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B24" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="6"/>
       <c r="H24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B25" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="5"/>
       <c r="E25" s="3"/>
       <c r="F25" s="7"/>
       <c r="H25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B26" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="5"/>
       <c r="E26" s="3"/>
       <c r="F26" s="6"/>
       <c r="H26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B27" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="5"/>
       <c r="E27" s="3"/>
       <c r="F27" s="6"/>
       <c r="H27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B28" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="7"/>
       <c r="H28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B29" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="6"/>
       <c r="H29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B30" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="6"/>
       <c r="H30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B31" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="6"/>
       <c r="H31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B32" s="15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="16"/>
       <c r="E32" s="8"/>
       <c r="F32" s="9"/>
       <c r="H32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B33" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="1"/>
       <c r="H33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Derniere version 06/03 17h30 excel
</commit_message>
<xml_diff>
--- a/Chezjombi/Fonctionnalite.xlsx
+++ b/Chezjombi/Fonctionnalite.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISEN\Desktop\Java\Chez_jombi\Chezjombi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivier\Documents\ISEN\M1\S2\Java\chez_jombi\Chezjombi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8709"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21945" windowHeight="8708"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
   <si>
     <t xml:space="preserve">Client </t>
   </si>
@@ -38,118 +38,124 @@
     <t xml:space="preserve">Patron </t>
   </si>
   <si>
+    <t>Boire</t>
+  </si>
+  <si>
+    <t>Jouer</t>
+  </si>
+  <si>
+    <t>Commander</t>
+  </si>
+  <si>
+    <t>Se battre</t>
+  </si>
+  <si>
+    <t>Aller WC</t>
+  </si>
+  <si>
+    <t>Payer</t>
+  </si>
+  <si>
+    <t>Draguer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmettre Argent </t>
+  </si>
+  <si>
+    <t>Offrir un Verre</t>
+  </si>
+  <si>
+    <t>Rendre Monaie</t>
+  </si>
+  <si>
+    <t>Gerer la fermeture</t>
+  </si>
+  <si>
+    <t>Gerer les stocks</t>
+  </si>
+  <si>
+    <t>que de l'eau</t>
+  </si>
+  <si>
+    <t>Se faire offrir</t>
+  </si>
+  <si>
+    <t>Se faire draguer</t>
+  </si>
+  <si>
+    <t>Preparer les commandes</t>
+  </si>
+  <si>
+    <t>Prendre une commande</t>
+  </si>
+  <si>
+    <t>Objectif :</t>
+  </si>
+  <si>
+    <t>Simulateur d'interraction dans un bar</t>
+  </si>
+  <si>
+    <t>Fonction/Personnage</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Serveur</t>
+  </si>
+  <si>
+    <t>Patron</t>
+  </si>
+  <si>
+    <t>Surnom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argent en poche </t>
+  </si>
+  <si>
+    <t>Charme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prenom </t>
+  </si>
+  <si>
+    <t>Attribu/Personnage</t>
+  </si>
+  <si>
+    <t>Boisson preferée</t>
+  </si>
+  <si>
+    <t>Sexe</t>
+  </si>
+  <si>
+    <t>Taille biceps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agilite </t>
+  </si>
+  <si>
+    <t>Boisson secours</t>
+  </si>
+  <si>
+    <t>Humain</t>
+  </si>
+  <si>
+    <t>Degres alcoolemie</t>
+  </si>
+  <si>
+    <t>Commun</t>
+  </si>
+  <si>
+    <t>Non Commun</t>
+  </si>
+  <si>
     <t>Parler</t>
   </si>
   <si>
-    <t>Boire</t>
-  </si>
-  <si>
-    <t>Jouer</t>
-  </si>
-  <si>
-    <t>Commander</t>
-  </si>
-  <si>
-    <t>Se battre</t>
-  </si>
-  <si>
-    <t>Aller WC</t>
-  </si>
-  <si>
-    <t>Payer</t>
-  </si>
-  <si>
-    <t>Draguer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transmettre Argent </t>
-  </si>
-  <si>
-    <t>Offrir un Verre</t>
-  </si>
-  <si>
-    <t>Rendre Monaie</t>
-  </si>
-  <si>
-    <t>Gerer la fermeture</t>
-  </si>
-  <si>
-    <t>Gerer les stocks</t>
-  </si>
-  <si>
-    <t>que de l'eau</t>
-  </si>
-  <si>
-    <t>Se faire offrir</t>
-  </si>
-  <si>
-    <t>Se faire draguer</t>
-  </si>
-  <si>
-    <t>Preparer les commandes</t>
-  </si>
-  <si>
-    <t>Prendre une commande</t>
-  </si>
-  <si>
-    <t>Objectif :</t>
-  </si>
-  <si>
-    <t>Simulateur d'interraction dans un bar</t>
-  </si>
-  <si>
-    <t>Fonction/Personnage</t>
-  </si>
-  <si>
-    <t>Client</t>
-  </si>
-  <si>
-    <t>Serveur</t>
-  </si>
-  <si>
-    <t>Patron</t>
-  </si>
-  <si>
-    <t>Surnom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Argent en poche </t>
-  </si>
-  <si>
-    <t>Charme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prenom </t>
-  </si>
-  <si>
-    <t>Attribu/Personnage</t>
-  </si>
-  <si>
-    <t>Boisson preferée</t>
-  </si>
-  <si>
-    <t>Sexe</t>
-  </si>
-  <si>
-    <t>Taille biceps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">agilite </t>
-  </si>
-  <si>
-    <t>Boisson secours</t>
-  </si>
-  <si>
-    <t>Humain</t>
-  </si>
-  <si>
-    <t>Degres alcoolemie</t>
-  </si>
-  <si>
-    <t>Commun</t>
-  </si>
-  <si>
-    <t>Non Commun</t>
+    <t>abstract</t>
+  </si>
+  <si>
+    <t>Servir à boire</t>
   </si>
 </sst>
 </file>
@@ -401,9 +407,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -414,6 +417,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,393 +734,412 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H33"/>
+  <dimension ref="B1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="21.15234375" customWidth="1"/>
-    <col min="3" max="3" width="11.07421875" customWidth="1"/>
-    <col min="8" max="8" width="18.61328125" customWidth="1"/>
+    <col min="2" max="2" width="21.1328125" customWidth="1"/>
+    <col min="3" max="3" width="11.06640625" customWidth="1"/>
+    <col min="8" max="8" width="18.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B4" s="18" t="s">
-        <v>4</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B4" s="17" t="s">
+        <v>41</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="6"/>
       <c r="H4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B5" s="14" t="s">
-        <v>5</v>
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B5" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="6"/>
       <c r="H5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B6" s="14" t="s">
-        <v>6</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B6" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
       <c r="H6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B7" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="6"/>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B8" s="13" t="s">
         <v>7</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="7"/>
-      <c r="H7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B8" s="14" t="s">
-        <v>8</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="6"/>
       <c r="H8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B9" s="14" t="s">
-        <v>9</v>
+        <v>39</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B9" s="13" t="s">
+        <v>8</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="5"/>
       <c r="F9" s="7"/>
       <c r="H9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B10" s="14" t="s">
-        <v>10</v>
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B10" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="7"/>
       <c r="H10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B11" s="14" t="s">
-        <v>13</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B11" s="13" t="s">
+        <v>12</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="5"/>
       <c r="E11" s="3"/>
       <c r="F11" s="6"/>
       <c r="H11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B12" s="14" t="s">
-        <v>11</v>
+        <v>39</v>
+      </c>
+      <c r="I11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B12" s="13" t="s">
+        <v>10</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="5"/>
       <c r="E12" s="3"/>
       <c r="F12" s="6"/>
       <c r="H12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B13" s="14" t="s">
-        <v>12</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B13" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="3"/>
       <c r="E13" s="5"/>
       <c r="F13" s="6"/>
       <c r="H13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B14" s="14" t="s">
-        <v>14</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B14" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="3"/>
       <c r="F14" s="7"/>
       <c r="H14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B15" s="14" t="s">
-        <v>16</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B15" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="3"/>
       <c r="F15" s="7"/>
       <c r="H15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B16" s="14" t="s">
-        <v>15</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B16" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="3"/>
       <c r="F16" s="7"/>
       <c r="H16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B17" s="14" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B17" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
       <c r="H17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B18" s="14" t="s">
-        <v>19</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B18" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="5"/>
       <c r="F18" s="7"/>
       <c r="H18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B19" s="14" t="s">
-        <v>20</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B19" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="3"/>
       <c r="F19" s="6"/>
       <c r="H19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="16"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B20" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="15"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="9"/>
       <c r="H20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B23" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B23" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="E23" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B24" s="14" t="s">
-        <v>31</v>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B24" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="6"/>
       <c r="H24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B25" s="14" t="s">
-        <v>28</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B25" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="5"/>
       <c r="E25" s="3"/>
       <c r="F25" s="7"/>
       <c r="H25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B26" s="14" t="s">
-        <v>33</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B26" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="5"/>
       <c r="E26" s="3"/>
       <c r="F26" s="6"/>
       <c r="H26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B27" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B27" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="5"/>
       <c r="E27" s="3"/>
       <c r="F27" s="6"/>
       <c r="H27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B28" s="14" t="s">
-        <v>29</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B28" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="7"/>
       <c r="H28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B29" s="14" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B29" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="6"/>
       <c r="H29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B30" s="14" t="s">
-        <v>35</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B30" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="6"/>
       <c r="H30" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B31" s="14" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B31" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="6"/>
       <c r="H31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="15" t="s">
-        <v>30</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B32" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="C32" s="8"/>
-      <c r="D32" s="16"/>
+      <c r="D32" s="15"/>
       <c r="E32" s="8"/>
       <c r="F32" s="9"/>
       <c r="H32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B33" s="20" t="s">
-        <v>39</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B33" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="H33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise a jour des fonctions
</commit_message>
<xml_diff>
--- a/Chezjombi/Fonctionnalite.xlsx
+++ b/Chezjombi/Fonctionnalite.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivier\Documents\ISEN\M1\S2\Java\chez_jombi\Chezjombi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISEN\Desktop\Java\Chez_jombi\Chezjombi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21945" windowHeight="8708"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8709"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>Gerer les stocks</t>
   </si>
   <si>
-    <t>que de l'eau</t>
-  </si>
-  <si>
     <t>Se faire offrir</t>
   </si>
   <si>
@@ -155,7 +152,10 @@
     <t>abstract</t>
   </si>
   <si>
-    <t>Servir à boire</t>
+    <t>a tester</t>
+  </si>
+  <si>
+    <t>que de l'eau manque exeception pointeur null</t>
   </si>
 </sst>
 </file>
@@ -734,38 +734,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L33"/>
+  <dimension ref="B1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="21.1328125" customWidth="1"/>
-    <col min="3" max="3" width="11.06640625" customWidth="1"/>
-    <col min="8" max="8" width="18.59765625" customWidth="1"/>
+    <col min="2" max="2" width="21.15234375" customWidth="1"/>
+    <col min="3" max="3" width="11.07421875" customWidth="1"/>
+    <col min="4" max="4" width="40.53515625" customWidth="1"/>
+    <col min="8" max="8" width="18.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>22</v>
       </c>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
       <c r="F1" s="20"/>
     </row>
-    <row r="2" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="L2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>0</v>
@@ -780,39 +777,41 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B4" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="6"/>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B5" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="6"/>
       <c r="H5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B6" s="13" t="s">
         <v>5</v>
       </c>
@@ -821,10 +820,10 @@
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
       <c r="H6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B7" s="13" t="s">
         <v>6</v>
       </c>
@@ -833,13 +832,13 @@
       <c r="E7" s="3"/>
       <c r="F7" s="6"/>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
@@ -848,13 +847,13 @@
       <c r="E8" s="3"/>
       <c r="F8" s="6"/>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B9" s="13" t="s">
         <v>8</v>
       </c>
@@ -863,13 +862,13 @@
       <c r="E9" s="5"/>
       <c r="F9" s="7"/>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B10" s="13" t="s">
         <v>9</v>
       </c>
@@ -878,10 +877,10 @@
       <c r="E10" s="5"/>
       <c r="F10" s="7"/>
       <c r="H10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B11" s="13" t="s">
         <v>12</v>
       </c>
@@ -890,13 +889,13 @@
       <c r="E11" s="3"/>
       <c r="F11" s="6"/>
       <c r="H11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B12" s="13" t="s">
         <v>10</v>
       </c>
@@ -905,10 +904,10 @@
       <c r="E12" s="3"/>
       <c r="F12" s="6"/>
       <c r="H12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B13" s="13" t="s">
         <v>11</v>
       </c>
@@ -917,10 +916,10 @@
       <c r="E13" s="5"/>
       <c r="F13" s="6"/>
       <c r="H13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B14" s="13" t="s">
         <v>13</v>
       </c>
@@ -929,10 +928,10 @@
       <c r="E14" s="3"/>
       <c r="F14" s="7"/>
       <c r="H14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B15" s="13" t="s">
         <v>15</v>
       </c>
@@ -941,10 +940,10 @@
       <c r="E15" s="3"/>
       <c r="F15" s="7"/>
       <c r="H15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B16" s="13" t="s">
         <v>14</v>
       </c>
@@ -953,193 +952,193 @@
       <c r="E16" s="3"/>
       <c r="F16" s="7"/>
       <c r="H16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B17" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
       <c r="H17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B18" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="5"/>
       <c r="F18" s="7"/>
       <c r="H18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B19" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="3"/>
       <c r="F19" s="6"/>
       <c r="H19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="9"/>
       <c r="H20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B23" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>2</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B24" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="6"/>
       <c r="H24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B25" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="5"/>
       <c r="E25" s="3"/>
       <c r="F25" s="7"/>
       <c r="H25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B26" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="5"/>
       <c r="E26" s="3"/>
       <c r="F26" s="6"/>
       <c r="H26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B27" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="5"/>
       <c r="E27" s="3"/>
       <c r="F27" s="6"/>
       <c r="H27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B28" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="7"/>
       <c r="H28" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B29" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="6"/>
       <c r="H29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B30" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="6"/>
       <c r="H30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B31" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="6"/>
       <c r="H31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B32" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="15"/>
       <c r="E32" s="8"/>
       <c r="F32" s="9"/>
       <c r="H32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B33" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="H33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>